<commit_message>
Added documentations for UI, Schema, and Chapter
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
-  <si>
-    <t>eDyscalculia: Database Schema</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
   <si>
     <t>tbl_account</t>
   </si>
@@ -185,9 +182,6 @@
     <t>scoretype_date</t>
   </si>
   <si>
-    <t>tbl_related_topic</t>
-  </si>
-  <si>
     <t>topic_id</t>
   </si>
   <si>
@@ -216,6 +210,39 @@
   </si>
   <si>
     <t>dyscalculia_date</t>
+  </si>
+  <si>
+    <t>tbl_chapter</t>
+  </si>
+  <si>
+    <t>chapter_id</t>
+  </si>
+  <si>
+    <t>chapter_slog</t>
+  </si>
+  <si>
+    <t>chapter_text</t>
+  </si>
+  <si>
+    <t>chapter_date</t>
+  </si>
+  <si>
+    <t>tbl_lesson</t>
+  </si>
+  <si>
+    <t>eDyscalculia: Database Schema (dyscalculia_db)</t>
+  </si>
+  <si>
+    <t>lesson_id</t>
+  </si>
+  <si>
+    <t>tbl_lvl</t>
+  </si>
+  <si>
+    <t>lvl_id</t>
+  </si>
+  <si>
+    <t>lvl_date</t>
   </si>
 </sst>
 </file>
@@ -275,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,6 +361,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
@@ -405,7 +437,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -417,8 +449,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,12 +459,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -445,71 +474,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="7" builtinId="39"/>
     <cellStyle name="40% - Accent5" xfId="8" builtinId="47"/>
@@ -517,6 +561,7 @@
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Accent3" xfId="6" builtinId="37"/>
+    <cellStyle name="Accent5" xfId="11" builtinId="45"/>
     <cellStyle name="Accent6" xfId="9" builtinId="49"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -798,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T27"/>
+  <dimension ref="B2:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,540 +861,695 @@
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
     <col min="13" max="13" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="M5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="27"/>
-      <c r="T5" s="27"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="M5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="11" t="s">
         <v>4</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>5</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="11"/>
-      <c r="J6" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="30"/>
+      <c r="J6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="21"/>
       <c r="M6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="11"/>
       <c r="S6" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T6" s="11"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="K7" s="12"/>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13" t="s">
+      <c r="T7" s="12"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="M7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="T7" s="13"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="I9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="I9" s="23" t="s">
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="11" t="s">
+      <c r="M10" s="11"/>
+      <c r="N10" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="P10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="14"/>
       <c r="I11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15" t="s">
+      <c r="M11" s="30"/>
+      <c r="N11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="P11" s="15"/>
+      <c r="Q11" s="30"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
+      <c r="B13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14" s="11"/>
-      <c r="I14" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="28"/>
+      <c r="I14" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="26"/>
       <c r="K14" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L14" s="11"/>
       <c r="M14" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P14" s="11"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="13"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="12"/>
       <c r="M15" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P15" s="14"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
-      <c r="G17" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="G17" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="26"/>
+      <c r="K18" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="29"/>
+      <c r="M18" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="16" t="s">
+      <c r="N18" s="29"/>
+      <c r="O18" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="L18" s="17"/>
-      <c r="M18" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="P18" s="26"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="12"/>
+      <c r="O19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="13"/>
-      <c r="M19" t="s">
-        <v>9</v>
-      </c>
+      <c r="P19" s="14"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
-      <c r="I21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="12"/>
+      <c r="I21" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F22" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="11"/>
       <c r="I22" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J22" s="11"/>
       <c r="K22" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L22" s="11"/>
       <c r="M22" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N22" s="11"/>
       <c r="O22" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="R22" s="11"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="14"/>
-      <c r="I23" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="R23" s="13"/>
+      <c r="I23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="12"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="G25" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="12"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="33"/>
+      <c r="F30" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
+  <mergeCells count="79">
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G17:P17"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
@@ -1363,49 +1563,15 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N10:O10"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="I9:P9"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="G17:M17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the upload helper on server by froala. Updated the Database Schema.
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ph2150105\Downloads\TIP - eDyscalculia Mobile App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project\javascript\ionic\dyscalculia_app\materials\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new schema" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
   <si>
     <t>tbl_account</t>
   </si>
@@ -243,6 +244,39 @@
   </si>
   <si>
     <t>lvl_date</t>
+  </si>
+  <si>
+    <t>int(11)</t>
+  </si>
+  <si>
+    <t>lesson _title</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>lesson_content</t>
+  </si>
+  <si>
+    <t>lesson_date</t>
+  </si>
+  <si>
+    <t>lesson _slog</t>
+  </si>
+  <si>
+    <t>lesson_status</t>
+  </si>
+  <si>
+    <t>chapter_status</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int(11) </t>
+  </si>
+  <si>
+    <t>with comment (0 = inactive, 1 = active)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +485,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,84 +508,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
@@ -845,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,48 +915,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="M5" s="20" t="s">
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="M5" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -921,36 +971,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="21" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="21"/>
+      <c r="K6" s="32"/>
       <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11" t="s">
+      <c r="R6" s="15"/>
+      <c r="S6" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="11"/>
+      <c r="T6" s="15"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -965,57 +1015,57 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="12"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="16"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" s="12"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="16"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="I9" s="22" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="I9" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1030,30 +1080,30 @@
       <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="19"/>
+      <c r="J10" s="36"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11" t="s">
+      <c r="M10" s="15"/>
+      <c r="N10" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11" t="s">
+      <c r="O10" s="15"/>
+      <c r="P10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1068,14 +1118,14 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="14"/>
-      <c r="I11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="14"/>
+      <c r="F11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="I11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="22"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
@@ -1083,33 +1133,33 @@
         <v>7</v>
       </c>
       <c r="M11" s="30"/>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="14"/>
+      <c r="O11" s="22"/>
       <c r="P11" s="30" t="s">
         <v>8</v>
       </c>
       <c r="Q11" s="30"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1121,30 +1171,30 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11" t="s">
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="26" t="s">
+      <c r="H14" s="15"/>
+      <c r="I14" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="11" t="s">
+      <c r="J14" s="25"/>
+      <c r="K14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11" t="s">
+      <c r="N14" s="15"/>
+      <c r="O14" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="11"/>
+      <c r="P14" s="15"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1156,50 +1206,50 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14" t="s">
+      <c r="F15" s="34"/>
+      <c r="G15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="12" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="14"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="22"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="G17" s="27" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="G17" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1220,22 +1270,22 @@
       <c r="H18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="26"/>
-      <c r="K18" s="28" t="s">
+      <c r="J18" s="25"/>
+      <c r="K18" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="29"/>
-      <c r="M18" s="28" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="29"/>
-      <c r="O18" s="26" t="s">
+      <c r="N18" s="28"/>
+      <c r="O18" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="26"/>
+      <c r="P18" s="25"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1256,44 +1306,44 @@
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12" t="s">
+      <c r="I19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12" t="s">
+      <c r="L19" s="16"/>
+      <c r="M19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="N19" s="12"/>
-      <c r="O19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19" s="14"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="22"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="I21" s="31" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="I21" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1308,30 +1358,30 @@
       <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="I22" s="11" t="s">
+      <c r="G22" s="15"/>
+      <c r="I22" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11" t="s">
+      <c r="J22" s="15"/>
+      <c r="K22" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11" t="s">
+      <c r="L22" s="15"/>
+      <c r="M22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11" t="s">
+      <c r="N22" s="15"/>
+      <c r="O22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11" t="s">
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="11"/>
+      <c r="R22" s="15"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1346,48 +1396,48 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="14"/>
-      <c r="I23" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12" t="s">
+      <c r="F23" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="I23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12" t="s">
+      <c r="L23" s="16"/>
+      <c r="M23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12" t="s">
+      <c r="N23" s="16"/>
+      <c r="O23" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="R23" s="12"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="16"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="G25" s="32" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="G25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1402,22 +1452,22 @@
       <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11" t="s">
+      <c r="H26" s="15"/>
+      <c r="I26" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11" t="s">
+      <c r="J26" s="15"/>
+      <c r="K26" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11" t="s">
+      <c r="L26" s="15"/>
+      <c r="M26" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="11"/>
+      <c r="N26" s="15"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1432,32 +1482,32 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12" t="s">
+      <c r="G27" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12" t="s">
+      <c r="J27" s="16"/>
+      <c r="K27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="N27" s="12"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="16"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -1466,14 +1516,14 @@
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="11" t="s">
+      <c r="E30" s="14"/>
+      <c r="F30" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="11"/>
+      <c r="G30" s="15"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1482,41 +1532,56 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="12"/>
+      <c r="D31" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
@@ -1533,45 +1598,840 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:T37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="M5" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="M6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="15"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="16"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="I9" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="I11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="30"/>
+      <c r="N11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="22"/>
+      <c r="P11" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="30"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="15"/>
+      <c r="I14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="P14" s="15"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="34"/>
+      <c r="G15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="22"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="G17" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="N18" s="25"/>
+      <c r="O18" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="T18" s="25"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="22"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="I21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="I22" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="I23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="16"/>
+      <c r="O23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="16"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="G25" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="R26" s="15"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="22"/>
+      <c r="K27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27" s="16"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="35" spans="2:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B35" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="89">
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K18:L18"/>
     <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="O19:P19"/>
     <mergeCell ref="M19:N19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="G17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="F11:G11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="N11:O11"/>
     <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the chapter route and added the docs for the chapter endpoints.
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="85">
   <si>
     <t>tbl_account</t>
   </si>
@@ -261,9 +261,6 @@
     <t>lesson_date</t>
   </si>
   <si>
-    <t>lesson _slog</t>
-  </si>
-  <si>
     <t>lesson_status</t>
   </si>
   <si>
@@ -277,6 +274,12 @@
   </si>
   <si>
     <t>with comment (0 = inactive, 1 = active)</t>
+  </si>
+  <si>
+    <t>lesson_slog</t>
+  </si>
+  <si>
+    <t>Default: 0</t>
   </si>
 </sst>
 </file>
@@ -517,11 +520,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,46 +530,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
@@ -577,31 +557,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
@@ -895,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,48 +918,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="M5" s="31" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="M5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -979,10 +982,10 @@
         <v>5</v>
       </c>
       <c r="I6" s="15"/>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="25"/>
       <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1047,25 +1050,25 @@
       <c r="T7" s="16"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="29" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="I9" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1080,15 +1083,15 @@
       <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="36"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
@@ -1118,48 +1121,48 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="I11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="22"/>
+      <c r="F11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="I11" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="18"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="22" t="s">
+      <c r="M11" s="28"/>
+      <c r="N11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="30"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="28"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1179,10 +1182,10 @@
         <v>17</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="15" t="s">
         <v>34</v>
       </c>
@@ -1206,14 +1209,14 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="22" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="16" t="s">
         <v>22</v>
       </c>
@@ -1222,34 +1225,34 @@
         <v>6</v>
       </c>
       <c r="L15" s="16"/>
-      <c r="M15" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="22"/>
+      <c r="M15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="18"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="G17" s="26" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="G17" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1270,22 +1273,22 @@
       <c r="H18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="27" t="s">
+      <c r="J18" s="27"/>
+      <c r="K18" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="28"/>
-      <c r="M18" s="27" t="s">
+      <c r="L18" s="34"/>
+      <c r="M18" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="28"/>
-      <c r="O18" s="25" t="s">
+      <c r="N18" s="34"/>
+      <c r="O18" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="25"/>
+      <c r="P18" s="27"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1318,32 +1321,32 @@
         <v>22</v>
       </c>
       <c r="N19" s="16"/>
-      <c r="O19" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19" s="22"/>
+      <c r="O19" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="18"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="I21" s="19" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="I21" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1396,10 +1399,10 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="22"/>
+      <c r="F23" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="18"/>
       <c r="I23" s="16" t="s">
         <v>6</v>
       </c>
@@ -1422,22 +1425,22 @@
       <c r="R23" s="16"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="G25" s="18" t="s">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="G25" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1500,14 +1503,14 @@
       <c r="N27" s="16"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -1516,10 +1519,10 @@
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="14"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="15" t="s">
         <v>72</v>
       </c>
@@ -1543,12 +1546,63 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G17:P17"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
@@ -1565,63 +1619,12 @@
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G17:P17"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1633,7 +1636,7 @@
   <dimension ref="B2:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,48 +1655,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="M5" s="31" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="M5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1716,10 +1719,10 @@
         <v>5</v>
       </c>
       <c r="I6" s="15"/>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="25"/>
       <c r="M6" s="10" t="s">
         <v>27</v>
       </c>
@@ -1784,25 +1787,25 @@
       <c r="T7" s="16"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="I9" s="29" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="I9" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
@@ -1817,15 +1820,15 @@
       <c r="E10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="36"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
@@ -1855,48 +1858,48 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="22"/>
-      <c r="I11" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="22"/>
+      <c r="F11" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="I11" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="18"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="22" t="s">
+      <c r="M11" s="28"/>
+      <c r="N11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="22"/>
-      <c r="P11" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="30"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="28"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
@@ -1916,10 +1919,10 @@
         <v>17</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="25"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="15" t="s">
         <v>34</v>
       </c>
@@ -1943,14 +1946,14 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="22" t="s">
+      <c r="F15" s="20"/>
+      <c r="G15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="16" t="s">
         <v>22</v>
       </c>
@@ -1959,38 +1962,38 @@
         <v>6</v>
       </c>
       <c r="L15" s="16"/>
-      <c r="M15" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="22"/>
+      <c r="M15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="18"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="G17" s="39" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="G17" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2011,30 +2014,30 @@
       <c r="H18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25" t="s">
+      <c r="J18" s="27"/>
+      <c r="K18" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25" t="s">
+      <c r="L18" s="27"/>
+      <c r="M18" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="N18" s="27"/>
+      <c r="O18" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25" t="s">
+      <c r="R18" s="27"/>
+      <c r="S18" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="T18" s="25"/>
+      <c r="T18" s="27"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -2071,36 +2074,36 @@
         <v>22</v>
       </c>
       <c r="P19" s="16"/>
-      <c r="Q19" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="T19" s="22"/>
+      <c r="Q19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="18"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="I21" s="19" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="I21" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
@@ -2153,10 +2156,10 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="22"/>
+      <c r="F23" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="18"/>
       <c r="I23" s="16" t="s">
         <v>6</v>
       </c>
@@ -2179,12 +2182,12 @@
       <c r="R23" s="16"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
       <c r="G25" s="40" t="s">
         <v>62</v>
       </c>
@@ -2230,7 +2233,7 @@
       </c>
       <c r="N26" s="15"/>
       <c r="O26" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P26" s="15"/>
       <c r="Q26" s="15" t="s">
@@ -2255,10 +2258,10 @@
         <v>6</v>
       </c>
       <c r="H27" s="16"/>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="22"/>
+      <c r="J27" s="18"/>
       <c r="K27" s="16" t="s">
         <v>22</v>
       </c>
@@ -2267,24 +2270,24 @@
         <v>22</v>
       </c>
       <c r="N27" s="16"/>
-      <c r="O27" s="22" t="s">
+      <c r="O27" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="P27" s="22"/>
+      <c r="P27" s="18"/>
       <c r="Q27" s="16" t="s">
         <v>8</v>
       </c>
       <c r="R27" s="16"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
@@ -2293,10 +2296,10 @@
       <c r="C30" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="14"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="15" t="s">
         <v>72</v>
       </c>
@@ -2318,110 +2321,37 @@
       </c>
       <c r="G31" s="16"/>
     </row>
-    <row r="35" spans="2:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B35" s="41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="22" t="s">
+    <row r="35" spans="2:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="B35" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="18"/>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="G37" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="G17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="B5:K5"/>
@@ -2432,6 +2362,85 @@
     <mergeCell ref="O6:P6"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="S6:T6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="G17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Lesson route done. Create doc for lesson then into difficulty route
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="87">
   <si>
     <t>tbl_account</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Default: 0</t>
+  </si>
+  <si>
+    <t>question_content</t>
+  </si>
+  <si>
+    <t>question_status</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,90 +527,97 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
@@ -898,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,48 +931,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="M5" s="24" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="M5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -974,36 +987,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="18"/>
+      <c r="J6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="35"/>
       <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15" t="s">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15" t="s">
+      <c r="R6" s="18"/>
+      <c r="S6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="15"/>
+      <c r="T6" s="18"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1018,57 +1031,57 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="16"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="19"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" s="16"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="19"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="I9" s="26" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="I9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1083,30 +1096,30 @@
       <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="23"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15" t="s">
+      <c r="M10" s="18"/>
+      <c r="N10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="15"/>
+      <c r="Q10" s="18"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1121,48 +1134,48 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="I11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="18"/>
+      <c r="F11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="I11" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="25"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="N11" s="18" t="s">
+      <c r="M11" s="33"/>
+      <c r="N11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="28"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="33"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1174,30 +1187,30 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15" t="s">
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="27" t="s">
+      <c r="H14" s="18"/>
+      <c r="I14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="15" t="s">
+      <c r="J14" s="28"/>
+      <c r="K14" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15" t="s">
+      <c r="L14" s="18"/>
+      <c r="M14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15" t="s">
+      <c r="N14" s="18"/>
+      <c r="O14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="15"/>
+      <c r="P14" s="18"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1209,50 +1222,50 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="18" t="s">
+      <c r="F15" s="37"/>
+      <c r="G15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="19"/>
+      <c r="M15" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="25"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="G17" s="32" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="G17" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1273,22 +1286,22 @@
       <c r="H18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="33" t="s">
+      <c r="J18" s="28"/>
+      <c r="K18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="34"/>
-      <c r="M18" s="33" t="s">
+      <c r="L18" s="31"/>
+      <c r="M18" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="34"/>
-      <c r="O18" s="27" t="s">
+      <c r="N18" s="31"/>
+      <c r="O18" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="27"/>
+      <c r="P18" s="28"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1309,44 +1322,44 @@
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16" t="s">
+      <c r="I19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16" t="s">
+      <c r="L19" s="19"/>
+      <c r="M19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="N19" s="16"/>
-      <c r="O19" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19" s="18"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="25"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="I21" s="35" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="I21" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1361,30 +1374,30 @@
       <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="I22" s="15" t="s">
+      <c r="G22" s="18"/>
+      <c r="I22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15" t="s">
+      <c r="J22" s="18"/>
+      <c r="K22" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15" t="s">
+      <c r="L22" s="18"/>
+      <c r="M22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15" t="s">
+      <c r="N22" s="18"/>
+      <c r="O22" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15" t="s">
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="15"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1399,48 +1412,48 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="18"/>
-      <c r="I23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
+      <c r="F23" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="I23" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16" t="s">
+      <c r="L23" s="19"/>
+      <c r="M23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16" t="s">
+      <c r="N23" s="19"/>
+      <c r="O23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="R23" s="16"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="19"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="G25" s="36" t="s">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="G25" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1455,22 +1468,22 @@
       <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15" t="s">
+      <c r="H26" s="18"/>
+      <c r="I26" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15" t="s">
+      <c r="J26" s="18"/>
+      <c r="K26" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15" t="s">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="15"/>
+      <c r="N26" s="18"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1485,32 +1498,32 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16" t="s">
+      <c r="G27" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16" t="s">
+      <c r="J27" s="19"/>
+      <c r="K27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="N27" s="16"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="19"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -1519,14 +1532,14 @@
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="15"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1535,41 +1548,56 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="16"/>
+      <c r="D31" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
@@ -1586,45 +1614,30 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1635,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,7 +1658,7 @@
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
@@ -1655,48 +1668,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="M5" s="24" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="M5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1711,36 +1724,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="18"/>
+      <c r="J6" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="35"/>
       <c r="M6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15" t="s">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15" t="s">
+      <c r="R6" s="18"/>
+      <c r="S6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="15"/>
+      <c r="T6" s="18"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1755,57 +1768,57 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16" t="s">
+      <c r="G7" s="19"/>
+      <c r="H7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="16"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="19"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" s="16"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="19"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="I9" s="26" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="I9" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
@@ -1820,30 +1833,30 @@
       <c r="E10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="23"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15" t="s">
+      <c r="M10" s="18"/>
+      <c r="N10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15" t="s">
+      <c r="O10" s="18"/>
+      <c r="P10" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="15"/>
+      <c r="Q10" s="18"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1858,83 +1871,71 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="I11" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="18"/>
+      <c r="F11" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="I11" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="25"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="N11" s="18" t="s">
+      <c r="M11" s="33"/>
+      <c r="N11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="18"/>
-      <c r="P11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="28"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="33"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="I14" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="27"/>
-      <c r="K14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15" t="s">
+      <c r="F14" s="18"/>
+      <c r="G14" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="15"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1944,56 +1945,48 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="18"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="25"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="G17" s="41" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="G17" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="41"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2014,30 +2007,30 @@
       <c r="H18" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27" t="s">
+      <c r="J18" s="28"/>
+      <c r="K18" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="N18" s="27"/>
-      <c r="O18" s="33" t="s">
+      <c r="N18" s="28"/>
+      <c r="O18" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="27" t="s">
+      <c r="P18" s="31"/>
+      <c r="Q18" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27" t="s">
+      <c r="R18" s="28"/>
+      <c r="S18" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="T18" s="27"/>
+      <c r="T18" s="28"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -2058,97 +2051,104 @@
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16" t="s">
+      <c r="I19" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16" t="s">
+      <c r="L19" s="19"/>
+      <c r="M19" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16" t="s">
+      <c r="N19" s="19"/>
+      <c r="O19" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="18" t="s">
+      <c r="P19" s="19"/>
+      <c r="Q19" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="T19" s="18"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T19" s="25"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="I21" s="35" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="K21" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="G22" s="18"/>
+      <c r="H22" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="16"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15" t="s">
+      <c r="L22" s="18"/>
+      <c r="M22" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15" t="s">
+      <c r="N22" s="18"/>
+      <c r="O22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15" t="s">
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15" t="s">
+      <c r="R22" s="18"/>
+      <c r="S22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="15"/>
+      <c r="T22" s="18"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -2156,52 +2156,56 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="18"/>
-      <c r="I23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16" t="s">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16" t="s">
+      <c r="H23" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="25"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16" t="s">
+      <c r="N23" s="19"/>
+      <c r="O23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="R23" s="16"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="T23" s="19"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="G25" s="40" t="s">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="G25" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="40"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="40"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
@@ -2216,30 +2220,30 @@
       <c r="E26" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15" t="s">
+      <c r="H26" s="18"/>
+      <c r="I26" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15" t="s">
+      <c r="J26" s="18"/>
+      <c r="K26" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15" t="s">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15" t="s">
+      <c r="N26" s="18"/>
+      <c r="O26" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15" t="s">
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="R26" s="15"/>
+      <c r="R26" s="18"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2254,40 +2258,40 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="18" t="s">
+      <c r="G27" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="19"/>
+      <c r="I27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="18"/>
-      <c r="K27" s="16" t="s">
+      <c r="J27" s="25"/>
+      <c r="K27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16" t="s">
+      <c r="L27" s="19"/>
+      <c r="M27" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="N27" s="16"/>
-      <c r="O27" s="18" t="s">
+      <c r="N27" s="19"/>
+      <c r="O27" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="R27" s="16"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27" s="19"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
@@ -2296,14 +2300,14 @@
       <c r="C30" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="15"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -2312,14 +2316,14 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="16"/>
+      <c r="D31" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="19"/>
     </row>
     <row r="35" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B35" s="13" t="s">
@@ -2327,10 +2331,10 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="25"/>
       <c r="D36" t="s">
         <v>82</v>
       </c>
@@ -2339,10 +2343,10 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="18"/>
+      <c r="C37" s="25"/>
       <c r="D37" t="s">
         <v>82</v>
       </c>
@@ -2351,7 +2355,78 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="89">
+  <mergeCells count="86">
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="K21:T21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="G17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="B13:L13"/>
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="B5:K5"/>
@@ -2367,80 +2442,6 @@
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="G17:T17"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="Q19:R19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on the question route. and updated the schema of the question_range (needs to update the question_range route queries).
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="103">
   <si>
     <t>tbl_account</t>
   </si>
@@ -328,6 +328,12 @@
   </si>
   <si>
     <t>question_range_date</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -543,7 +549,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,117 +585,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1006,48 +1015,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="M5" s="30" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="M5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1062,36 +1071,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="31" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="31"/>
+      <c r="K6" s="42"/>
       <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21" t="s">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21" t="s">
+      <c r="R6" s="25"/>
+      <c r="S6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="21"/>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1106,57 +1115,57 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="26"/>
+      <c r="J7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="26"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="O7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22" t="s">
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="22"/>
+      <c r="T7" s="26"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="I9" s="32" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="I9" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1171,30 +1180,30 @@
       <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="28" t="s">
+      <c r="I10" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="29"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21" t="s">
+      <c r="M10" s="25"/>
+      <c r="N10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21" t="s">
+      <c r="O10" s="25"/>
+      <c r="P10" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="21"/>
+      <c r="Q10" s="25"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1209,48 +1218,48 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="I11" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="24"/>
+      <c r="G11" s="32"/>
+      <c r="I11" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="32"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="34" t="s">
+      <c r="L11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="34"/>
-      <c r="N11" s="24" t="s">
+      <c r="M11" s="40"/>
+      <c r="N11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="24"/>
-      <c r="P11" s="34" t="s">
+      <c r="O11" s="32"/>
+      <c r="P11" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="34"/>
+      <c r="Q11" s="40"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1262,30 +1271,30 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="33" t="s">
+      <c r="H14" s="25"/>
+      <c r="I14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="21" t="s">
+      <c r="J14" s="35"/>
+      <c r="K14" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21" t="s">
+      <c r="L14" s="25"/>
+      <c r="M14" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21" t="s">
+      <c r="N14" s="25"/>
+      <c r="O14" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="21"/>
+      <c r="P14" s="25"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1297,50 +1306,50 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="24" t="s">
+      <c r="F15" s="44"/>
+      <c r="G15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="24"/>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="32"/>
+      <c r="I15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24" t="s">
+      <c r="J15" s="26"/>
+      <c r="K15" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="26"/>
+      <c r="M15" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="24"/>
+      <c r="P15" s="32"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="G17" s="38" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="G17" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1361,22 +1370,22 @@
       <c r="H18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="39" t="s">
+      <c r="J18" s="35"/>
+      <c r="K18" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="39" t="s">
+      <c r="L18" s="38"/>
+      <c r="M18" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="40"/>
-      <c r="O18" s="33" t="s">
+      <c r="N18" s="38"/>
+      <c r="O18" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="33"/>
+      <c r="P18" s="35"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1397,44 +1406,44 @@
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22" t="s">
+      <c r="I19" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22" t="s">
+      <c r="L19" s="26"/>
+      <c r="M19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N19" s="22"/>
-      <c r="O19" s="24" t="s">
+      <c r="N19" s="26"/>
+      <c r="O19" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="24"/>
+      <c r="P19" s="32"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="I21" s="41" t="s">
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="I21" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1449,30 +1458,30 @@
       <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="I22" s="21" t="s">
+      <c r="G22" s="25"/>
+      <c r="I22" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21" t="s">
+      <c r="J22" s="25"/>
+      <c r="K22" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21" t="s">
+      <c r="L22" s="25"/>
+      <c r="M22" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21" t="s">
+      <c r="N22" s="25"/>
+      <c r="O22" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="21"/>
-      <c r="Q22" s="21" t="s">
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="21"/>
+      <c r="R22" s="25"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1487,48 +1496,48 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="I23" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22" t="s">
+      <c r="G23" s="32"/>
+      <c r="I23" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22" t="s">
+      <c r="L23" s="26"/>
+      <c r="M23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22" t="s">
+      <c r="N23" s="26"/>
+      <c r="O23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22" t="s">
+      <c r="P23" s="26"/>
+      <c r="Q23" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="22"/>
+      <c r="R23" s="26"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="G25" s="42" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="G25" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1543,22 +1552,22 @@
       <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
+      <c r="H26" s="25"/>
+      <c r="I26" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21" t="s">
+      <c r="J26" s="25"/>
+      <c r="K26" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21" t="s">
+      <c r="L26" s="25"/>
+      <c r="M26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="21"/>
+      <c r="N26" s="25"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1573,32 +1582,32 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22" t="s">
+      <c r="G27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22" t="s">
+      <c r="J27" s="26"/>
+      <c r="K27" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22" t="s">
+      <c r="L27" s="26"/>
+      <c r="M27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="22"/>
+      <c r="N27" s="26"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -1607,14 +1616,14 @@
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="44"/>
-      <c r="F30" s="21" t="s">
+      <c r="E30" s="24"/>
+      <c r="F30" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="21"/>
+      <c r="G30" s="25"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1623,41 +1632,56 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22" t="s">
+      <c r="D31" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="22"/>
+      <c r="G31" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="B13:P13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
@@ -1674,45 +1698,30 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="B13:P13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1723,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,48 +1753,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="M5" s="30" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="M5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1800,36 +1809,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="31" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="31"/>
+      <c r="K6" s="42"/>
       <c r="M6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21" t="s">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21" t="s">
+      <c r="R6" s="25"/>
+      <c r="S6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="21"/>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1844,66 +1853,66 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22" t="s">
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="26"/>
+      <c r="J7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="22"/>
+      <c r="K7" s="26"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="22" t="s">
+      <c r="O7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22" t="s">
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="22"/>
+      <c r="T7" s="26"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="I9" s="52" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="I9" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1912,33 +1921,33 @@
       <c r="E10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="53" t="s">
+      <c r="G10" s="31"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="21" t="s">
+      <c r="J10" s="50"/>
+      <c r="K10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21" t="s">
+      <c r="L10" s="25"/>
+      <c r="M10" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21" t="s">
+      <c r="N10" s="25"/>
+      <c r="O10" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21" t="s">
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1953,32 +1962,32 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="I11" s="22" t="s">
+      <c r="G11" s="32"/>
+      <c r="I11" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22" t="s">
+      <c r="J11" s="26"/>
+      <c r="K11" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22" t="s">
+      <c r="L11" s="26"/>
+      <c r="M11" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22" t="s">
+      <c r="N11" s="26"/>
+      <c r="O11" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22" t="s">
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="26"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1990,114 +1999,114 @@
       <c r="D12" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="51">
+      <c r="E12" s="22">
         <v>0.9</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="50"/>
+      <c r="G12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21" t="s">
+      <c r="E14" s="25"/>
+      <c r="F14" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21" t="s">
+      <c r="G14" s="25"/>
+      <c r="H14" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21" t="s">
+      <c r="I14" s="25"/>
+      <c r="J14" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="21"/>
-      <c r="L14" s="50"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22" t="s">
+      <c r="G15" s="26"/>
+      <c r="H15" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22" t="s">
+      <c r="I15" s="26"/>
+      <c r="J15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="O15" s="17"/>
+      <c r="K15" s="26"/>
+      <c r="O15" s="16"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2106,33 +2115,33 @@
       <c r="C18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21" t="s">
+      <c r="E18" s="25"/>
+      <c r="F18" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="21"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="I18" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21" t="s">
+      <c r="J18" s="25"/>
+      <c r="K18" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21" t="s">
+      <c r="L18" s="25"/>
+      <c r="M18" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21" t="s">
+      <c r="N18" s="25"/>
+      <c r="O18" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="21"/>
+      <c r="P18" s="25"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -2141,64 +2150,93 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="22"/>
+      <c r="D19" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="26"/>
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="24" t="s">
+      <c r="I19" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="44"/>
+      <c r="K19" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24" t="s">
+      <c r="L19" s="32"/>
+      <c r="M19" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="24"/>
+      <c r="P19" s="32"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>101</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="H21" s="47" t="s">
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="H21" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-      <c r="Q21" s="47"/>
-      <c r="R21" s="47"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="47"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="52"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="52"/>
+      <c r="S21" s="52"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="52"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="10" t="s">
@@ -2216,30 +2254,30 @@
       <c r="I22" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33" t="s">
+      <c r="K22" s="35"/>
+      <c r="L22" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33" t="s">
+      <c r="M22" s="35"/>
+      <c r="N22" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="O22" s="33"/>
-      <c r="P22" s="39" t="s">
+      <c r="O22" s="35"/>
+      <c r="P22" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="33" t="s">
+      <c r="Q22" s="38"/>
+      <c r="R22" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33" t="s">
+      <c r="S22" s="35"/>
+      <c r="T22" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="U22" s="33"/>
+      <c r="U22" s="35"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -2263,54 +2301,52 @@
       <c r="I23" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22" t="s">
+      <c r="J23" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22" t="s">
+      <c r="M23" s="26"/>
+      <c r="N23" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22" t="s">
+      <c r="O23" s="26"/>
+      <c r="P23" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="24" t="s">
+      <c r="Q23" s="26"/>
+      <c r="R23" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24" t="s">
+      <c r="S23" s="32"/>
+      <c r="T23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="U23" s="24"/>
+      <c r="U23" s="32"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="K25" s="41" t="s">
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="I25" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
@@ -2319,41 +2355,37 @@
       <c r="C26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21" t="s">
+      <c r="F26" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="43"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="21" t="s">
+      <c r="G26" s="25"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21" t="s">
+      <c r="J26" s="24"/>
+      <c r="K26" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21" t="s">
+      <c r="L26" s="24"/>
+      <c r="M26" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21" t="s">
+      <c r="N26" s="24"/>
+      <c r="O26" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21" t="s">
+      <c r="P26" s="24"/>
+      <c r="Q26" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="T26" s="21"/>
+      <c r="R26" s="24"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2368,56 +2400,53 @@
       <c r="E27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="L27" s="26"/>
+      <c r="M27" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" s="22"/>
-      <c r="O27" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="R27" s="22"/>
-      <c r="S27" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="T27" s="22"/>
+      <c r="R27" s="26"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="G29" s="46" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="G29" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
@@ -2432,30 +2461,30 @@
       <c r="E30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21" t="s">
+      <c r="H30" s="25"/>
+      <c r="I30" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21" t="s">
+      <c r="J30" s="25"/>
+      <c r="K30" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21" t="s">
+      <c r="L30" s="25"/>
+      <c r="M30" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21" t="s">
+      <c r="N30" s="25"/>
+      <c r="O30" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21" t="s">
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="R30" s="21"/>
+      <c r="R30" s="25"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -2470,95 +2499,96 @@
       <c r="E31" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="24" t="s">
+      <c r="G31" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="26"/>
+      <c r="I31" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="J31" s="24"/>
-      <c r="K31" s="22" t="s">
+      <c r="J31" s="32"/>
+      <c r="K31" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22" t="s">
+      <c r="L31" s="26"/>
+      <c r="M31" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="22"/>
-      <c r="O31" s="24" t="s">
+      <c r="N31" s="26"/>
+      <c r="O31" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="22" t="s">
+      <c r="P31" s="32"/>
+      <c r="Q31" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="R31" s="22"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="45" t="s">
+      <c r="R31" s="26"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="43" t="s">
+      <c r="D34" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="44"/>
-      <c r="F34" s="21" t="s">
+      <c r="E34" s="24"/>
+      <c r="F34" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="21"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22" t="s">
+      <c r="D35" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="22"/>
-    </row>
-    <row r="39" spans="2:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="G35" s="26"/>
+    </row>
+    <row r="39" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="24" t="s">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="24"/>
+      <c r="C40" s="32"/>
       <c r="D40" t="s">
         <v>82</v>
       </c>
       <c r="G40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="24"/>
+      <c r="C41" s="32"/>
       <c r="D41" t="s">
         <v>82</v>
       </c>
@@ -2567,7 +2597,85 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="103">
+  <mergeCells count="102">
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="I25:R25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="G29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="H21:U21"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="B17:P17"/>
@@ -2592,85 +2700,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K25:T25"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="H21:U21"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="G29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on the question route. Lists is done
</commit_message>
<xml_diff>
--- a/materials/documentation/eDyscalculia Database Schema.xlsx
+++ b/materials/documentation/eDyscalculia Database Schema.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="104">
   <si>
     <t>tbl_account</t>
   </si>
@@ -315,9 +315,6 @@
     <t>question_range_slog</t>
   </si>
   <si>
-    <t>question_range_text</t>
-  </si>
-  <si>
     <t>pre-test</t>
   </si>
   <si>
@@ -334,6 +331,12 @@
   </si>
   <si>
     <t>a</t>
+  </si>
+  <si>
+    <t>question_range_from</t>
+  </si>
+  <si>
+    <t>question_range_to</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -605,11 +608,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -617,46 +617,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="8" applyBorder="1" applyAlignment="1">
@@ -665,40 +644,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1015,48 +1015,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="M5" s="41" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="M5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1071,36 +1071,36 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="42" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="42"/>
+      <c r="K6" s="34"/>
       <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="25" t="s">
+      <c r="O6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25" t="s">
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25" t="s">
+      <c r="R6" s="24"/>
+      <c r="S6" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="25"/>
+      <c r="T6" s="24"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1115,57 +1115,57 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26" t="s">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="26"/>
+      <c r="K7" s="25"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26" t="s">
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="26"/>
+      <c r="T7" s="25"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="I9" s="39" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="I9" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
@@ -1188,22 +1188,22 @@
       <c r="I10" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="46"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25" t="s">
+      <c r="M10" s="24"/>
+      <c r="N10" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25" t="s">
+      <c r="O10" s="24"/>
+      <c r="P10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="25"/>
+      <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1218,48 +1218,48 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="I11" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="32"/>
+      <c r="G11" s="27"/>
+      <c r="I11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="27"/>
       <c r="K11" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="L11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="40"/>
-      <c r="N11" s="32" t="s">
+      <c r="M11" s="37"/>
+      <c r="N11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="32"/>
-      <c r="P11" s="40" t="s">
+      <c r="O11" s="27"/>
+      <c r="P11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="Q11" s="40"/>
+      <c r="Q11" s="37"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -1271,30 +1271,30 @@
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="35" t="s">
+      <c r="H14" s="24"/>
+      <c r="I14" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="25" t="s">
+      <c r="J14" s="36"/>
+      <c r="K14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25" t="s">
+      <c r="L14" s="24"/>
+      <c r="M14" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25" t="s">
+      <c r="N14" s="24"/>
+      <c r="O14" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="P14" s="25"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1306,50 +1306,50 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="32" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="26" t="s">
+      <c r="H15" s="27"/>
+      <c r="I15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="26"/>
-      <c r="M15" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32" t="s">
+      <c r="J15" s="25"/>
+      <c r="K15" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="25"/>
+      <c r="M15" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="32"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="G17" s="36" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="G17" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="41"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1370,22 +1370,22 @@
       <c r="H18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="35"/>
-      <c r="K18" s="37" t="s">
+      <c r="J18" s="36"/>
+      <c r="K18" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="38"/>
-      <c r="M18" s="37" t="s">
+      <c r="L18" s="43"/>
+      <c r="M18" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="38"/>
-      <c r="O18" s="35" t="s">
+      <c r="N18" s="43"/>
+      <c r="O18" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="35"/>
+      <c r="P18" s="36"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -1406,44 +1406,44 @@
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26" t="s">
+      <c r="I19" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26" t="s">
+      <c r="L19" s="25"/>
+      <c r="M19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N19" s="26"/>
-      <c r="O19" s="32" t="s">
+      <c r="N19" s="25"/>
+      <c r="O19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="32"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="I21" s="29" t="s">
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="I21" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="29"/>
-      <c r="R21" s="29"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
+      <c r="N21" s="44"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
@@ -1458,30 +1458,30 @@
       <c r="E22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="I22" s="25" t="s">
+      <c r="G22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25" t="s">
+      <c r="J22" s="24"/>
+      <c r="K22" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25" t="s">
+      <c r="L22" s="24"/>
+      <c r="M22" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25" t="s">
+      <c r="N22" s="24"/>
+      <c r="O22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25" t="s">
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="R22" s="25"/>
+      <c r="R22" s="24"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -1496,48 +1496,48 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="32"/>
-      <c r="I23" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26" t="s">
+      <c r="G23" s="27"/>
+      <c r="I23" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26" t="s">
+      <c r="L23" s="25"/>
+      <c r="M23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26" t="s">
+      <c r="N23" s="25"/>
+      <c r="O23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="26" t="s">
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="26"/>
+      <c r="R23" s="25"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="G25" s="28" t="s">
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="G25" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
@@ -1552,22 +1552,22 @@
       <c r="E26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25" t="s">
+      <c r="H26" s="24"/>
+      <c r="I26" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25" t="s">
+      <c r="J26" s="24"/>
+      <c r="K26" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25" t="s">
+      <c r="L26" s="24"/>
+      <c r="M26" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="25"/>
+      <c r="N26" s="24"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -1582,32 +1582,32 @@
       <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26" t="s">
+      <c r="G27" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26" t="s">
+      <c r="J27" s="25"/>
+      <c r="K27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26" t="s">
+      <c r="L27" s="25"/>
+      <c r="M27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="26"/>
+      <c r="N27" s="25"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
@@ -1616,14 +1616,14 @@
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25" t="s">
+      <c r="E30" s="47"/>
+      <c r="F30" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="25"/>
+      <c r="G30" s="24"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1632,23 +1632,74 @@
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26" t="s">
+      <c r="D31" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="G25:N25"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="I21:R21"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G17:P17"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="I9:Q9"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
@@ -1665,63 +1716,12 @@
     <mergeCell ref="N10:O10"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="I9:Q9"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G17:P17"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="I21:R21"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="G25:N25"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1730,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U41"/>
+  <dimension ref="B2:V41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,51 +1752,51 @@
     <col min="17" max="17" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="M5" s="41" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="M5" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1809,38 +1809,38 @@
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="25"/>
-      <c r="J6" s="42" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="42"/>
+      <c r="K6" s="34"/>
       <c r="M6" s="10" t="s">
         <v>27</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="25" t="s">
+      <c r="O6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25" t="s">
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25" t="s">
+      <c r="R6" s="24"/>
+      <c r="S6" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="25"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="T6" s="24"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1853,62 +1853,64 @@
       <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26" t="s">
+      <c r="I7" s="25"/>
+      <c r="J7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="26"/>
+      <c r="K7" s="25"/>
       <c r="M7" t="s">
         <v>6</v>
       </c>
       <c r="N7" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="26" t="s">
+      <c r="O7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26" t="s">
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="26"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="T7" s="25"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="I9" s="49" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="I9" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-      <c r="P9" s="49"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
@@ -1926,30 +1928,34 @@
       </c>
       <c r="G10" s="31"/>
       <c r="H10" s="18"/>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="25" t="s">
+      <c r="J10" s="52"/>
+      <c r="K10" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25" t="s">
+      <c r="L10" s="24"/>
+      <c r="M10" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="N10" s="24"/>
+      <c r="O10" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1962,48 +1968,52 @@
       <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="32"/>
-      <c r="I11" s="26" t="s">
+      <c r="G11" s="27"/>
+      <c r="I11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26" t="s">
+      <c r="J11" s="25"/>
+      <c r="K11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26" t="s">
+      <c r="L11" s="25"/>
+      <c r="M11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26" t="s">
+      <c r="N11" s="25"/>
+      <c r="O11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26" t="s">
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="26"/>
-      <c r="T11" s="26"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="s">
         <v>97</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
       </c>
       <c r="E12" s="22">
         <v>0.9</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12" s="16"/>
       <c r="I12" s="16"/>
@@ -2014,68 +2024,68 @@
       <c r="O12" s="16"/>
       <c r="P12" s="21"/>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="25" t="s">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25" t="s">
+      <c r="I14" s="24"/>
+      <c r="J14" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26" t="s">
+      <c r="E15" s="25"/>
+      <c r="F15" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26" t="s">
+      <c r="G15" s="25"/>
+      <c r="H15" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26" t="s">
+      <c r="I15" s="25"/>
+      <c r="J15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="26"/>
+      <c r="K15" s="25"/>
       <c r="O15" s="16"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -2090,23 +2100,23 @@
       <c r="R16" s="22"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -2115,33 +2125,33 @@
       <c r="C18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="25"/>
+      <c r="G18" s="24"/>
       <c r="H18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25" t="s">
+      <c r="J18" s="24"/>
+      <c r="K18" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25" t="s">
+      <c r="L18" s="24"/>
+      <c r="M18" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25" t="s">
+      <c r="N18" s="24"/>
+      <c r="O18" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="25"/>
+      <c r="P18" s="24"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -2150,33 +2160,33 @@
       <c r="C19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="26"/>
+      <c r="D19" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="25"/>
       <c r="H19" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" s="44"/>
-      <c r="K19" s="32" t="s">
+      <c r="I19" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32" t="s">
+      <c r="L19" s="27"/>
+      <c r="M19" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="P19" s="32"/>
+      <c r="P19" s="27"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -2198,39 +2208,39 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="H21" s="52" t="s">
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="H21" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="52"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="52"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
@@ -2254,30 +2264,30 @@
       <c r="I22" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="35" t="s">
+      <c r="J22" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35" t="s">
+      <c r="K22" s="36"/>
+      <c r="L22" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35" t="s">
+      <c r="M22" s="36"/>
+      <c r="N22" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="O22" s="35"/>
-      <c r="P22" s="37" t="s">
+      <c r="O22" s="36"/>
+      <c r="P22" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="Q22" s="38"/>
-      <c r="R22" s="35" t="s">
+      <c r="Q22" s="43"/>
+      <c r="R22" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35" t="s">
+      <c r="S22" s="36"/>
+      <c r="T22" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="U22" s="35"/>
+      <c r="U22" s="36"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -2301,52 +2311,52 @@
       <c r="I23" t="s">
         <v>6</v>
       </c>
-      <c r="J23" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26" t="s">
+      <c r="J23" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26" t="s">
+      <c r="M23" s="25"/>
+      <c r="N23" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26" t="s">
+      <c r="O23" s="25"/>
+      <c r="P23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="32" t="s">
+      <c r="Q23" s="25"/>
+      <c r="R23" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32" t="s">
+      <c r="S23" s="27"/>
+      <c r="T23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="U23" s="32"/>
+      <c r="U23" s="27"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="I25" s="29" t="s">
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="I25" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
-      <c r="P25" s="29"/>
-      <c r="Q25" s="29"/>
-      <c r="R25" s="29"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
@@ -2361,31 +2371,31 @@
       <c r="E26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="25"/>
+      <c r="G26" s="24"/>
       <c r="H26" s="18"/>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="24"/>
-      <c r="K26" s="23" t="s">
+      <c r="J26" s="47"/>
+      <c r="K26" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="L26" s="24"/>
-      <c r="M26" s="23" t="s">
+      <c r="L26" s="47"/>
+      <c r="M26" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="N26" s="24"/>
-      <c r="O26" s="23" t="s">
+      <c r="N26" s="47"/>
+      <c r="O26" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="23" t="s">
+      <c r="P26" s="47"/>
+      <c r="Q26" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="R26" s="24"/>
+      <c r="R26" s="47"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -2400,53 +2410,53 @@
       <c r="E27" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="26"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="19"/>
-      <c r="I27" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26" t="s">
+      <c r="I27" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26" t="s">
+      <c r="L27" s="25"/>
+      <c r="M27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26" t="s">
+      <c r="N27" s="25"/>
+      <c r="O27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="26" t="s">
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R27" s="26"/>
+      <c r="R27" s="25"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="G29" s="54" t="s">
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="G29" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="54"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
@@ -2461,30 +2471,30 @@
       <c r="E30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25" t="s">
+      <c r="H30" s="24"/>
+      <c r="I30" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25" t="s">
+      <c r="J30" s="24"/>
+      <c r="K30" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25" t="s">
+      <c r="L30" s="24"/>
+      <c r="M30" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25" t="s">
+      <c r="N30" s="24"/>
+      <c r="O30" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25" t="s">
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="R30" s="25"/>
+      <c r="R30" s="24"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -2499,40 +2509,40 @@
       <c r="E31" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="32" t="s">
+      <c r="G31" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="J31" s="32"/>
-      <c r="K31" s="26" t="s">
+      <c r="J31" s="27"/>
+      <c r="K31" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26" t="s">
+      <c r="L31" s="25"/>
+      <c r="M31" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="N31" s="26"/>
-      <c r="O31" s="32" t="s">
+      <c r="N31" s="25"/>
+      <c r="O31" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="26" t="s">
+      <c r="P31" s="27"/>
+      <c r="Q31" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="R31" s="26"/>
+      <c r="R31" s="25"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="48"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
@@ -2541,14 +2551,14 @@
       <c r="C34" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25" t="s">
+      <c r="E34" s="47"/>
+      <c r="F34" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
@@ -2557,14 +2567,14 @@
       <c r="C35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26" t="s">
+      <c r="D35" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="26"/>
+      <c r="G35" s="25"/>
     </row>
     <row r="39" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
@@ -2572,10 +2582,10 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="32"/>
+      <c r="C40" s="27"/>
       <c r="D40" t="s">
         <v>82</v>
       </c>
@@ -2585,10 +2595,10 @@
       <c r="J40" s="21"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="32"/>
+      <c r="C41" s="27"/>
       <c r="D41" t="s">
         <v>82</v>
       </c>
@@ -2597,20 +2607,79 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="102">
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
+  <mergeCells count="104">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="I9:V9"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B17:P17"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="T10:V10"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="M5:T5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="H21:U21"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="T23:U23"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="O19:P19"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="I25:R25"/>
@@ -2630,76 +2699,19 @@
     <mergeCell ref="O31:P31"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="O30:P30"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="H21:U21"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="T23:U23"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="B2:H3"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="M5:T5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B17:P17"/>
-    <mergeCell ref="I9:T9"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>